<commit_message>
Update namespace and create course model
</commit_message>
<xml_diff>
--- a/test_models/courses.xlsx
+++ b/test_models/courses.xlsx
@@ -16,30 +16,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Яндекс лицей</t>
-  </si>
-  <si>
-    <t>Комампания яндекс в очередной раз проводит делает набор в ряды своих юных разработчиков.
-                        Бесплатное обучение проходит в течении 4 полугодии, в течении которых ученики получают хорошие
-                        знания языка програмирования Python.</t>
-  </si>
-  <si>
-    <t>../static/icon/Yandex_lyceum.jpg</t>
-  </si>
-  <si>
-    <t>GitHub</t>
-  </si>
-  <si>
-    <t>GitHub — это крупнейший веб-сервис для хостинга IT-проектов и их совместной разработки.
-                    Веб-сервис основан на системе контроля версий Git и разработан на Ruby on Rails и Erlang компанией
-                    GitHub, Inc (ранее Logical Awesome). Сервис бесплатен для проектов с открытым исходным кодом и (с
-                    2019 года) небольших частных проектов, предоставляя им все возможности (включая SSL), а для крупных
-                    корпоративных проектов предлагаются различные платные тарифные планы.</t>
-  </si>
-  <si>
-    <t>../static/icon/git.png</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Курсы</t>
+  </si>
+  <si>
+    <t>Яндекс Лицей</t>
+  </si>
+  <si>
+    <t>Обучение програмированию на языке Python на базе компании Яндекс.</t>
+  </si>
+  <si>
+    <t>icon/yandex.jpg</t>
+  </si>
+  <si>
+    <t>Онлайн обучение</t>
+  </si>
+  <si>
+    <t>Super-English</t>
+  </si>
+  <si>
+    <t>Изучение английского языка с нуля, до свободного общения вместе с Петровой Оксаной Сергеевной.</t>
+  </si>
+  <si>
+    <t>icon/English.jpg</t>
   </si>
 </sst>
 </file>
@@ -77,9 +77,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -381,43 +379,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="3" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1">
+        <v>43344</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43862</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>